<commit_message>
resolve problem of graph don't go to last vertice
</commit_message>
<xml_diff>
--- a/graph.xlsx
+++ b/graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davir\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davir\OneDrive\Área de Trabalho\Graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CEB9BF-815B-4178-B987-BD76A2C19B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E0804F-7A08-431D-A0F8-9A314FB9488D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0AE69268-5A23-49B0-A2B5-0AF3830B68F7}"/>
+    <workbookView xWindow="870" yWindow="3240" windowWidth="21600" windowHeight="11295" xr2:uid="{0AE69268-5A23-49B0-A2B5-0AF3830B68F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA96FCC2-90B3-4941-90E1-9163D16B5C9A}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +619,9 @@
       <c r="G5" s="6">
         <v>9</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
       <c r="I5" s="6">
         <v>23</v>
       </c>

</xml_diff>